<commit_message>
Use Config from ENV and repo tidy (#6)
* tidy up ro-crate builder:

* docstrings to RO-builder

* add handling for additional properties

* read mytardisconfig file

* modify abi-crate cli to accept schemas from config

* modify abi-crate cli to accept schemas from config

* updated print lab parser to use env config
</commit_message>
<xml_diff>
--- a/examples_for_test/print_lab_test/sampledata.xlsx
+++ b/examples_for_test/print_lab_test/sampledata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" state="visible" r:id="rId3"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="89">
   <si>
     <t xml:space="preserve">Sample name</t>
   </si>
@@ -203,15 +203,6 @@
     <t xml:space="preserve">Macrogen Illumina MiSeq</t>
   </si>
   <si>
-    <t xml:space="preserve">VCF/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vcf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00001-018-C0001-02-2C10.1-D-01</t>
-  </si>
-  <si>
     <t xml:space="preserve">Participant: Code</t>
   </si>
   <si>
@@ -303,24 +294,6 @@
   </si>
   <si>
     <t xml:space="preserve">QC from fastqc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/jlove/projects/ro_crate_mt_ingestions/test.txt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hg18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">file not listed in crate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">does/not/exist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hg2200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">file that does not exist</t>
   </si>
 </sst>
 </file>
@@ -558,7 +531,7 @@
   </sheetPr>
   <dimension ref="A1:S1002"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
     </sheetView>
   </sheetViews>
@@ -3786,10 +3759,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3889,39 +3862,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="I4" s="1" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2:H4" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2:H3" type="list">
       <formula1>Samples!$A$2:$A$65536</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3951,22 +3894,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>66</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>16</v>
@@ -3977,19 +3920,19 @@
         <v>33</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C2" s="6" t="n">
         <v>2</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -4022,30 +3965,30 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>32</v>
@@ -4054,21 +3997,21 @@
         <v>19</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>36</v>
@@ -4077,16 +4020,16 @@
         <v>19</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -4111,10 +4054,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4124,89 +4067,50 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>54</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H40" s="5"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H38" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H4" type="list">
-      <formula1>Samples!$A$2:$A$65536</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Updates following inital RO-Crate encryption implementation (#11)
* changes to test encryption

* changes to test encryption

* more elaborate print lab files

* graceful api failure

* graceful api failure

* update to crate and tar script

* updates following inital encryption implementation

* update lock
</commit_message>
<xml_diff>
--- a/examples_for_test/print_lab_test/sampledata.xlsx
+++ b/examples_for_test/print_lab_test/sampledata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" state="visible" r:id="rId3"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="89">
   <si>
     <t xml:space="preserve">Sample name</t>
   </si>
@@ -531,8 +531,8 @@
   </sheetPr>
   <dimension ref="A1:S1002"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S2" activeCellId="1" sqref="G2 S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3762,7 +3762,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="G2 A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3886,8 +3886,8 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3933,6 +3933,9 @@
       </c>
       <c r="F2" s="5" t="s">
         <v>67</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -3954,7 +3957,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="G2 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4056,8 +4059,8 @@
   </sheetPr>
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F21" activeCellId="1" sqref="G2 F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
update public key command (#13)
</commit_message>
<xml_diff>
--- a/examples_for_test/print_lab_test/sampledata.xlsx
+++ b/examples_for_test/print_lab_test/sampledata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" state="visible" r:id="rId3"/>
@@ -13,6 +13,7 @@
     <sheet name="Participants" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="Projects" sheetId="4" state="visible" r:id="rId6"/>
     <sheet name="Files" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="Groups" sheetId="6" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="_xlfn_CONCAT" vbProcedure="false"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="99">
   <si>
     <t xml:space="preserve">Sample name</t>
   </si>
@@ -83,6 +84,9 @@
     <t xml:space="preserve">Participant</t>
   </si>
   <si>
+    <t xml:space="preserve">Groups</t>
+  </si>
+  <si>
     <t xml:space="preserve">00001</t>
   </si>
   <si>
@@ -131,6 +135,9 @@
     <t xml:space="preserve">C0001</t>
   </si>
   <si>
+    <t xml:space="preserve">Group_general Group_sensitive,Group_specific </t>
+  </si>
+  <si>
     <t xml:space="preserve">02</t>
   </si>
   <si>
@@ -140,6 +147,9 @@
     <t xml:space="preserve">018</t>
   </si>
   <si>
+    <t xml:space="preserve">Group_general Group_sensitive</t>
+  </si>
+  <si>
     <t xml:space="preserve">Directory</t>
   </si>
   <si>
@@ -294,16 +304,38 @@
   </si>
   <si>
     <t xml:space="preserve">QC from fastqc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is_owner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">see_sensitive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">can_download</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group_general</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group_sensitive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group_specific</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -377,7 +409,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -403,6 +435,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -529,10 +565,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S1002"/>
+  <dimension ref="A1:T1002"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S2" activeCellId="1" sqref="G2 S2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S18" activeCellId="0" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -607,6 +643,9 @@
       <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="T1" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="str">
@@ -614,58 +653,61 @@
         <v>00001-016-C0001-01-2C10.1-D-01</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="R2" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="3" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -674,58 +716,61 @@
         <v>00001-018-C0001-02-2C10.1-D-01</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="S3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>33</v>
+      <c r="T3" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3762,7 +3807,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="G2 A4"/>
+      <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3775,57 +3820,57 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="I2" s="1" t="n">
         <f aca="false">TRUE()</f>
@@ -3834,28 +3879,28 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="H3" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="I3" s="1" t="n">
         <f aca="false">TRUE()</f>
@@ -3886,30 +3931,30 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>16</v>
@@ -3917,25 +3962,25 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C2" s="6" t="n">
         <v>2</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>32</v>
+        <v>70</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -3957,7 +4002,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="G2 B2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3968,71 +4013,71 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>76</v>
-      </c>
       <c r="E3" s="5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -4060,7 +4105,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F21" activeCellId="1" sqref="G2 F21"/>
+      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4070,48 +4115,128 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H38" s="5"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" s="7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7" t="b">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
update for seperation of repos (#15)
* add ACL data structures

* modify dataclasses for ACLs

* modify dataclasses for ACLs

* refactor of lab specific RO-Crate classes

* updates for ACLs

* mypy adjustments

* mypy adjustments

* moved medical condtion
</commit_message>
<xml_diff>
--- a/examples_for_test/print_lab_test/sampledata.xlsx
+++ b/examples_for_test/print_lab_test/sampledata.xlsx
@@ -438,7 +438,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -568,7 +568,7 @@
   <dimension ref="A1:T1002"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S18" activeCellId="0" sqref="S18"/>
+      <selection pane="topLeft" activeCell="R19" activeCellId="0" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4183,58 +4183,67 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="4" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="7" t="b">
+      <c r="B2" s="7" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="b">
+      <c r="C2" s="7" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D2" s="7" t="b">
+      <c r="D2" s="7" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="7" t="b">
+      <c r="B3" s="7" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C3" s="7" t="b">
+      <c r="C3" s="7" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D3" s="7" t="b">
+      <c r="D3" s="7" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B4" s="7" t="b">
+      <c r="B4" s="7" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="C4" s="7" t="b">
+      <c r="C4" s="7" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D4" s="7" t="b">
+      <c r="D4" s="7" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Move to external builder (#16)
* add ACL data structures

* modify dataclasses for ACLs

* modify dataclasses for ACLs

* refactor of lab specific RO-Crate classes

* updates for ACLs

* mypy adjustments

* mypy adjustments

* moved medical condtion

* changes from seperating RO-Crate builder

* update before splitting extraction repo

* delete old builder code
</commit_message>
<xml_diff>
--- a/examples_for_test/print_lab_test/sampledata.xlsx
+++ b/examples_for_test/print_lab_test/sampledata.xlsx
@@ -135,7 +135,7 @@
     <t xml:space="preserve">C0001</t>
   </si>
   <si>
-    <t xml:space="preserve">Group_general Group_sensitive,Group_specific </t>
+    <t xml:space="preserve">Group_general, Group_sensitive,Group_specific </t>
   </si>
   <si>
     <t xml:space="preserve">02</t>
@@ -147,7 +147,7 @@
     <t xml:space="preserve">018</t>
   </si>
   <si>
-    <t xml:space="preserve">Group_general Group_sensitive</t>
+    <t xml:space="preserve">Group_general, Group_sensitive</t>
   </si>
   <si>
     <t xml:space="preserve">Directory</t>
@@ -568,7 +568,7 @@
   <dimension ref="A1:T1002"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R19" activeCellId="0" sqref="R19"/>
+      <selection pane="topLeft" activeCell="P22" activeCellId="0" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
remove active directory lookup
</commit_message>
<xml_diff>
--- a/examples_for_test/print_lab_test/sampledata.xlsx
+++ b/examples_for_test/print_lab_test/sampledata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" state="visible" r:id="rId3"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="101">
   <si>
     <t xml:space="preserve">Sample name</t>
   </si>
@@ -267,6 +267,9 @@
     <t xml:space="preserve">NETWORK</t>
   </si>
   <si>
+    <t xml:space="preserve">jlov034</t>
+  </si>
+  <si>
     <t xml:space="preserve">13/NTA/69</t>
   </si>
   <si>
@@ -277,6 +280,9 @@
   </si>
   <si>
     <t xml:space="preserve">NETWORK2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptsa000</t>
   </si>
   <si>
     <t xml:space="preserve">Filepath</t>
@@ -426,16 +432,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -567,7 +573,7 @@
   </sheetPr>
   <dimension ref="A1:T1002"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="P22" activeCellId="0" sqref="P22"/>
     </sheetView>
   </sheetViews>
@@ -710,7 +716,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(B3,"-",R3,"-",S3,"-",G3,"-",I3,"-",P3,"-",Q3)</f>
         <v>00001-018-C0001-02-2C10.1-D-01</v>
@@ -3878,7 +3884,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -3938,45 +3944,45 @@
   <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="6" t="n">
+      <c r="C2" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>70</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -4001,92 +4007,86 @@
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="16.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="5" width="24.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="24.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="E2" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="F3" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>81</v>
-      </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C2:C3" type="list">
-      <formula1>#ref!</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -4114,49 +4114,49 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>85</v>
       </c>
+      <c r="B1" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="D1" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>88</v>
+      <c r="C2" s="4" t="s">
+        <v>90</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>88</v>
-      </c>
       <c r="D3" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H38" s="5"/>
+      <c r="H38" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4184,21 +4184,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B2" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -4215,7 +4215,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B3" s="7" t="n">
         <f aca="false">TRUE()</f>
@@ -4232,7 +4232,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B4" s="7" t="n">
         <f aca="false">FALSE()</f>

</xml_diff>

<commit_message>
Ids 779 remove active directory lookup from ro crate gener (#1)
* remove active directory lookup

* remove active directory lookup

* black changes to removed active directory lookup
</commit_message>
<xml_diff>
--- a/examples_for_test/print_lab_test/sampledata.xlsx
+++ b/examples_for_test/print_lab_test/sampledata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" state="visible" r:id="rId3"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="101">
   <si>
     <t xml:space="preserve">Sample name</t>
   </si>
@@ -267,6 +267,9 @@
     <t xml:space="preserve">NETWORK</t>
   </si>
   <si>
+    <t xml:space="preserve">jlov034</t>
+  </si>
+  <si>
     <t xml:space="preserve">13/NTA/69</t>
   </si>
   <si>
@@ -277,6 +280,9 @@
   </si>
   <si>
     <t xml:space="preserve">NETWORK2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptsa000</t>
   </si>
   <si>
     <t xml:space="preserve">Filepath</t>
@@ -426,16 +432,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -567,7 +573,7 @@
   </sheetPr>
   <dimension ref="A1:T1002"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="P22" activeCellId="0" sqref="P22"/>
     </sheetView>
   </sheetViews>
@@ -710,7 +716,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(B3,"-",R3,"-",S3,"-",G3,"-",I3,"-",P3,"-",Q3)</f>
         <v>00001-018-C0001-02-2C10.1-D-01</v>
@@ -3878,7 +3884,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -3938,45 +3944,45 @@
   <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="6" t="n">
+      <c r="C2" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>70</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -4001,92 +4007,86 @@
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="16.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="5" width="24.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="24.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="E2" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="F3" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>81</v>
-      </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C2:C3" type="list">
-      <formula1>#ref!</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -4114,49 +4114,49 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>85</v>
       </c>
+      <c r="B1" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="D1" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>88</v>
+      <c r="C2" s="4" t="s">
+        <v>90</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>88</v>
-      </c>
       <c r="D3" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H38" s="5"/>
+      <c r="H38" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4184,21 +4184,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B2" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -4215,7 +4215,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B3" s="7" t="n">
         <f aca="false">TRUE()</f>
@@ -4232,7 +4232,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B4" s="7" t="n">
         <f aca="false">FALSE()</f>

</xml_diff>

<commit_message>
update source on dataclasses that should contain children
</commit_message>
<xml_diff>
--- a/examples_for_test/print_lab_test/sampledata.xlsx
+++ b/examples_for_test/print_lab_test/sampledata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" state="visible" r:id="rId3"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="103">
   <si>
     <t xml:space="preserve">Sample name</t>
   </si>
@@ -201,6 +201,9 @@
     <t xml:space="preserve">00001-016-C0001-01-2C10.1-D-01</t>
   </si>
   <si>
+    <t xml:space="preserve">TRUE</t>
+  </si>
+  <si>
     <t xml:space="preserve">BAM/qc/</t>
   </si>
   <si>
@@ -211,6 +214,9 @@
   </si>
   <si>
     <t xml:space="preserve">Macrogen Illumina MiSeq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FALSE</t>
   </si>
   <si>
     <t xml:space="preserve">Participant: Code</t>
@@ -440,7 +446,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3812,8 +3818,8 @@
   </sheetPr>
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3878,26 +3884,25 @@
       <c r="H2" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="I2" s="1" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="I2" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>52</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>54</v>
@@ -3908,9 +3913,8 @@
       <c r="H3" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="I3" s="1" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="I3" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -3945,22 +3949,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>16</v>
@@ -3971,19 +3975,19 @@
         <v>34</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C2" s="5" t="n">
         <v>2</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>33</v>
@@ -4007,7 +4011,7 @@
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
     </sheetView>
   </sheetViews>
@@ -4019,71 +4023,71 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -4115,44 +4119,44 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>90</v>
-      </c>
       <c r="D3" s="4" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4184,21 +4188,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B2" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -4215,7 +4219,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B3" s="7" t="n">
         <f aca="false">TRUE()</f>
@@ -4232,7 +4236,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B4" s="7" t="n">
         <f aca="false">FALSE()</f>

</xml_diff>